<commit_message>
Task Assigned to Mr Umair
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7590" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7590" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Waqar Tanveer" sheetId="10" r:id="rId1"/>
@@ -23,12 +23,12 @@
     <sheet name="Hammad Zafar Tasks" sheetId="6" r:id="rId9"/>
     <sheet name="Abid Hussain Tasks" sheetId="1" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="392">
   <si>
     <t>Date</t>
   </si>
@@ -1246,6 +1246,9 @@
   </si>
   <si>
     <t>Worked on Teslar Project Create New User Consumer Account. Error handling and database dupilcation constraint fixed. Check here http://expertsvision.site/adduser . User name is : abid password: abid123.  Now manager can create new consumer account but error will be shown if email is used same for different consumers.  Email id must be nique. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on Omar Kanan Project </t>
   </si>
 </sst>
 </file>
@@ -2706,8 +2709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3149,8 +3152,8 @@
       <c r="A18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="23">
-        <v>0</v>
+      <c r="B18" s="23" t="s">
+        <v>391</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>

</xml_diff>